<commit_message>
fixing import publikasi lewat page
</commit_message>
<xml_diff>
--- a/public/file_ki/KI.xlsx
+++ b/public/file_ki/KI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Manajemen Data LPPM\Sistem-Manajemen-Data-LPPM\public\file_ki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5642A967-B1F7-4461-8940-AF4CB597D90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C74336-A551-434A-ACA0-F8C42D550B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C9ECFCB5-3E58-4BA0-88E7-74F84B807E7C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C0A108B-34A5-4BE4-AA5A-82E826D7D70A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Jenis HKI</t>
   </si>
   <si>
-    <t xml:space="preserve">Protoipe </t>
-  </si>
-  <si>
     <t>PATENT HOLDER</t>
   </si>
   <si>
@@ -285,30 +282,22 @@
   </si>
   <si>
     <t>Luaran PNLT/PKM</t>
+  </si>
+  <si>
+    <t>Prototipe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -320,12 +309,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.499984740745262"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -333,37 +322,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -700,16 +664,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A31F75D-AF0F-46C2-8A06-98997F142D98}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D4BDD2-B861-4DD2-93D4-B4595A3A380B}">
   <dimension ref="A1:CE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="67.6640625" customWidth="1"/>
@@ -776,7 +741,7 @@
     <col min="81" max="81" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:83" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,247 +757,242 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BO1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BP1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BR1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BS1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BT1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BU1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BV1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BW1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BX1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="BY1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CA1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CB1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CC1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CD1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CE1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="CE1" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{86DA259F-2C63-499B-8996-46A891628E00}">
-      <formula1>"Ada (Alat Tidak Diketahui),Ada ( Alat Ada dan Fungsi),Tidak Ada"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixing bug and optimize
add more filter ki,
delete prodi using prodi from data mahasiswa/dosen instead,
fix duplicate data  penulis/anggota when importing same data,
add id mahasiswa on main publikasi and ki, fix sidebar menu,
fix still href if just input link and not with number document,
fix if condition data has been deleted but want to add that same data again,
fix filtering : deleting query when and using selected choise insteed
</commit_message>
<xml_diff>
--- a/public/file_ki/KI.xlsx
+++ b/public/file_ki/KI.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Manajemen Data LPPM\Sistem-Manajemen-Data-LPPM\public\file_ki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B319CD92-BCC6-4F4B-A184-236189A193F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2965E29A-3671-48B8-A8CF-725441158819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C0A108B-34A5-4BE4-AA5A-82E826D7D70A}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{5C0A108B-34A5-4BE4-AA5A-82E826D7D70A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="KI" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
-  <si>
-    <t>No</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Application Number</t>
   </si>
@@ -65,9 +62,6 @@
     <t>Jabatan</t>
   </si>
   <si>
-    <t>Prodi</t>
-  </si>
-  <si>
     <t>PUBLICATION NUMBER</t>
   </si>
   <si>
@@ -95,115 +89,73 @@
     <t>Status Anggota 1</t>
   </si>
   <si>
-    <t>Prodi 1</t>
-  </si>
-  <si>
     <t>Anggota 2</t>
   </si>
   <si>
     <t>Status Anggota 2</t>
   </si>
   <si>
-    <t>Prodi 2</t>
-  </si>
-  <si>
     <t>Anggota 3</t>
   </si>
   <si>
     <t>Status Anggota 3</t>
   </si>
   <si>
-    <t>Prodi 3</t>
-  </si>
-  <si>
     <t>Anggota 4</t>
   </si>
   <si>
     <t>Status Anggota 4</t>
   </si>
   <si>
-    <t>Prodi 4</t>
-  </si>
-  <si>
     <t>Anggota 5</t>
   </si>
   <si>
     <t>Status Anggota 5</t>
   </si>
   <si>
-    <t>Prodi 5</t>
-  </si>
-  <si>
     <t>Anggota 6</t>
   </si>
   <si>
     <t>Status Anggota 6</t>
   </si>
   <si>
-    <t>Prodi 6</t>
-  </si>
-  <si>
     <t>Anggota 7</t>
   </si>
   <si>
     <t>Status Anggota 7</t>
   </si>
   <si>
-    <t>Prodi 7</t>
-  </si>
-  <si>
     <t>Anggota 8</t>
   </si>
   <si>
     <t>Status Anggota 8</t>
   </si>
   <si>
-    <t>Prodi 8</t>
-  </si>
-  <si>
     <t>Anggota 9</t>
   </si>
   <si>
     <t>Status Anggota 9</t>
   </si>
   <si>
-    <t>Prodi 9</t>
-  </si>
-  <si>
     <t>Nama Anggota 10</t>
   </si>
   <si>
     <t>Status Anggota 10</t>
   </si>
   <si>
-    <t>Prodi 10</t>
-  </si>
-  <si>
     <t>Nama Anggota 11</t>
   </si>
   <si>
     <t>Status Anggota 11</t>
   </si>
   <si>
-    <t>Prodi 11</t>
-  </si>
-  <si>
     <t>Nama Anggota 12</t>
   </si>
   <si>
     <t>Status Anggota 12</t>
   </si>
   <si>
-    <t>Prodi 12</t>
-  </si>
-  <si>
     <t>Link</t>
-  </si>
-  <si>
-    <t>Luaran TA / Non TA</t>
-  </si>
-  <si>
-    <t>Luaran PNLT/PKM</t>
   </si>
   <si>
     <t>Prototipe</t>
@@ -587,70 +539,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D4BDD2-B861-4DD2-93D4-B4595A3A380B}">
-  <dimension ref="A1:BE1"/>
+  <dimension ref="A1:AO1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BD5" sqref="BD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="67.6640625" customWidth="1"/>
-    <col min="6" max="7" width="38.44140625" customWidth="1"/>
-    <col min="8" max="8" width="28.109375" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" customWidth="1"/>
-    <col min="13" max="13" width="21.6640625" customWidth="1"/>
-    <col min="14" max="14" width="20.6640625" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="28.33203125" customWidth="1"/>
-    <col min="17" max="17" width="24.33203125" customWidth="1"/>
-    <col min="18" max="18" width="25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="67.6640625" customWidth="1"/>
+    <col min="5" max="6" width="38.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.109375" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="28.33203125" customWidth="1"/>
+    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="23" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.44140625" customWidth="1"/>
+    <col min="27" max="27" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,10 +604,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -773,54 +710,6 @@
       </c>
       <c r="AO1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>